<commit_message>
clean code - cap 1 and cap 2
</commit_message>
<xml_diff>
--- a/Basic-Intermediary-Advanced.xlsx
+++ b/Basic-Intermediary-Advanced.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t xml:space="preserve">ORIGINAL PHRASE</t>
   </si>
@@ -36,76 +36,73 @@
     <t xml:space="preserve">TRANSLATED WORD</t>
   </si>
   <si>
-    <t xml:space="preserve">moyen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">me parut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le moyen le plus efficace d’apprendre le japonais me parut d’enseigner le français.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enseigner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Au supermarché, je laissai une petite annonce : « Cours particuliers de français, prix intéressant ».</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annonce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le téléphone sonna le soir même. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sonna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rendez-vous fut pris pour le lendemain, dans un café d’Omote-Sando. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lendemain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je ne compris rien à son nom, lui non plus au mien. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raccrochant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">me rendis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En raccrochant, je me rendis compte que je ne savais pas à quoi je le reconnaîtrais, lui non plus. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">compte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Et comme je n’avais pas eu la présence d’esprit de lui demander son numéro, cela n’allait pas s’arranger. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">arranger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappellera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il me rappellera peut-être pour ce motif, pensai-je.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motif</t>
+    <t xml:space="preserve">or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">immortalité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gloire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">richesse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dignité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">respect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">espérance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">répos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fécondité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeunesse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enthousiasme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jaune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lumière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idéalisme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jalousie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sécurité</t>
   </si>
   <si>
     <t xml:space="preserve">PHRASE</t>
@@ -296,16 +293,17 @@
   <dimension ref="A1:AMJ50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="74.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="66.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -321,7 +319,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AMJ1" s="0"/>
+      <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
@@ -338,317 +336,300 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="E19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="0"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="0"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="0"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="0"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="0"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="B32" s="0"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="0"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="0"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="0"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
+      <c r="B36" s="0"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="B37" s="0"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="B38" s="0"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
+      <c r="B39" s="0"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
+      <c r="B40" s="0"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
+      <c r="B41" s="0"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
+      <c r="B42" s="0"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
+      <c r="B43" s="0"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
+      <c r="B44" s="0"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
+      <c r="B45" s="0"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
+      <c r="B46" s="0"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
+      <c r="B47" s="0"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
+      <c r="B48" s="0"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
+      <c r="B49" s="0"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
+      <c r="B50" s="0"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
@@ -681,16 +662,16 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -698,71 +679,71 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
working with kivymd and hotreloader
</commit_message>
<xml_diff>
--- a/Basic-Intermediary-Advanced.xlsx
+++ b/Basic-Intermediary-Advanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t xml:space="preserve">ORIGINAL PHRASE</t>
   </si>
@@ -36,75 +36,267 @@
     <t xml:space="preserve">TRANSLATED WORD</t>
   </si>
   <si>
+    <t xml:space="preserve">Le cours de l'or est très haut actuellement.</t>
+  </si>
+  <si>
     <t xml:space="preserve">or</t>
   </si>
   <si>
+    <t xml:space="preserve">The price of gold is very high at the moment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les légendes racontent l'immortalité des dieux.</t>
+  </si>
+  <si>
     <t xml:space="preserve">immortalité</t>
   </si>
   <si>
+    <t xml:space="preserve">Legends tell of the immortality of the gods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">immortality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On trouvera un moyen approprié de célébrer ta gloire.</t>
+  </si>
+  <si>
     <t xml:space="preserve">gloire</t>
   </si>
   <si>
+    <t xml:space="preserve">Nós ainda encontraremos um modo apropriado de celebrar a vossa glória.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'oncle d'Anne décède et elle hérite de sa richesse.</t>
+  </si>
+  <si>
     <t xml:space="preserve">richesse</t>
   </si>
   <si>
+    <t xml:space="preserve">O tio de Anne morre e ela herda sua fortuna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je pratiquerai ma profession avec conscience et dignité.</t>
+  </si>
+  <si>
     <t xml:space="preserve">dignité</t>
   </si>
   <si>
+    <t xml:space="preserve">Exercerei a minha profissão"com consciência e dignidade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dignity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le respect des anciens est la moindre des choses.</t>
+  </si>
+  <si>
     <t xml:space="preserve">respect</t>
   </si>
   <si>
+    <t xml:space="preserve">O respeito pelos mais velhos é a menor das coisas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au printemps, la nature est toute verte.</t>
+  </si>
+  <si>
     <t xml:space="preserve">vert</t>
   </si>
   <si>
+    <t xml:space="preserve">The countryside is very green in spring.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elle a l'espérance de connaître des jours meilleurs.</t>
+  </si>
+  <si>
     <t xml:space="preserve">espérance</t>
   </si>
   <si>
+    <t xml:space="preserve">She has hopes of seeing better days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon frère aime tellement la nature qu'il envisage de devenir garde forestier.</t>
+  </si>
+  <si>
     <t xml:space="preserve">nature</t>
   </si>
   <si>
+    <t xml:space="preserve">My brother likes nature so much that he's thinking of becoming a forest warden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tous ses muscles sont au repos.</t>
+  </si>
+  <si>
     <t xml:space="preserve">répos</t>
   </si>
   <si>
+    <t xml:space="preserve">All her muscles are at rest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'âge limite de la fécondité féminine recule de plus en plus.</t>
+  </si>
+  <si>
     <t xml:space="preserve">fécondité</t>
   </si>
   <si>
+    <t xml:space="preserve">The upper age limit for female fertility is being pushed back ever further.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fertility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La jeunesse, c'est l'avenir d'un pays.</t>
+  </si>
+  <si>
     <t xml:space="preserve">jeunesse</t>
   </si>
   <si>
+    <t xml:space="preserve">Young people are a country's future.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">youth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'orange est la couleur des Pays-Bas.</t>
+  </si>
+  <si>
     <t xml:space="preserve">orange</t>
   </si>
   <si>
+    <t xml:space="preserve">Orange is the color of Holland.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La responsable fait montre d'une grande énergie et a mené à bien plusieurs projets.</t>
+  </si>
+  <si>
     <t xml:space="preserve">energie</t>
   </si>
   <si>
+    <t xml:space="preserve">The supervisor shows a lot of energy and has brought many projects to a successful conclusion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son enthousiasme faisait plaisir à voir.</t>
+  </si>
+  <si>
     <t xml:space="preserve">enthousiasme</t>
   </si>
   <si>
+    <t xml:space="preserve">His enthusiasm was a pleasure to see.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enthusiasm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marion se raconte des histoires, elle a une imagination sans fin.</t>
+  </si>
+  <si>
     <t xml:space="preserve">imagination</t>
   </si>
   <si>
+    <t xml:space="preserve">Marion tells stories; she has a boundless imagination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Est-ce que tu aimes ma nouvelle robe jaune ?</t>
+  </si>
+  <si>
     <t xml:space="preserve">jaune</t>
   </si>
   <si>
+    <t xml:space="preserve">Do you like my new yellow dress?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nous constatons chaque jour les progrès de la science.</t>
+  </si>
+  <si>
     <t xml:space="preserve">science</t>
   </si>
   <si>
+    <t xml:space="preserve">We see advances in science every day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le maire a su ramener le calme dans ce quartier.</t>
+  </si>
+  <si>
     <t xml:space="preserve">calme</t>
   </si>
   <si>
+    <t xml:space="preserve">The mayor managed to restore calm in the neighbourhood.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sous cette lumière, la campagne est magnifique.</t>
+  </si>
+  <si>
     <t xml:space="preserve">lumière</t>
   </si>
   <si>
+    <t xml:space="preserve">In this light, the countryside is magnificent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courage, créativité, idéalisme, abnégation et engagement sont également nécessaires.</t>
+  </si>
+  <si>
     <t xml:space="preserve">idéalisme</t>
   </si>
   <si>
+    <t xml:space="preserve">Courage, creativity, idealism, selflessness and commitment are also needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idealism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez eu des crises de jalousie ou la suspicion.</t>
+  </si>
+  <si>
     <t xml:space="preserve">jalousie</t>
   </si>
   <si>
+    <t xml:space="preserve">Você tem tido crises de ciúme ou desconfiança.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jealousy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je circule dans une voiture blindée avec un service de sécurité.</t>
+  </si>
+  <si>
     <t xml:space="preserve">sécurité</t>
   </si>
   <si>
+    <t xml:space="preserve">Desloco-me num automóvel blindado com segurança.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">security</t>
+  </si>
+  <si>
     <t xml:space="preserve">PHRASE</t>
   </si>
   <si>
@@ -115,57 +307,6 @@
   </si>
   <si>
     <t xml:space="preserve">CONTEXT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Although “microservices” is a new term, the concepts that it represents have been around for long time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">around</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We finally built a new application with a completely different modern technology stack alongside the old one.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alongside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The old and the new application were only coupled via HTML links and via a shared database.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coupled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Except for the shared database, this is in essence a microservices approach.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have also realized how continuous delivery influences software architecture.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the reason for writing this book—a number of people have been pursuing a microservices approach for a long time, among them some very experienced architects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pursuing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical implementation strategies are not neglected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">neglected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These will help the interested reader to test their new knowledge practically and delve deeper into subjects that are of relevance to them.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delve</t>
   </si>
 </sst>
 </file>
@@ -175,7 +316,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -209,6 +350,13 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -256,7 +404,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,6 +421,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,6 +438,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF222222"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -292,21 +508,20 @@
   </sheetPr>
   <dimension ref="A1:AMJ50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A2:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="66.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="9.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -321,315 +536,478 @@
       </c>
       <c r="AMJ1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B18" s="3" t="s">
-        <v>7</v>
+        <v>65</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B19" s="3" t="s">
-        <v>20</v>
+        <v>69</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>72</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>76</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>80</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>84</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>88</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
-      <c r="B25" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
-      <c r="B27" s="0"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
-      <c r="B28" s="0"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="0"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
-      <c r="B30" s="0"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
-      <c r="B31" s="0"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
-      <c r="B32" s="0"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
-      <c r="B33" s="0"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
-      <c r="B34" s="0"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
-      <c r="B35" s="0"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
-      <c r="B36" s="0"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
-      <c r="B37" s="0"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
-      <c r="B38" s="0"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
-      <c r="B39" s="0"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
-      <c r="B40" s="0"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
-      <c r="B41" s="0"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
-      <c r="B42" s="0"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
-      <c r="B43" s="0"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
-      <c r="B44" s="0"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
-      <c r="B45" s="0"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
-      <c r="B46" s="0"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
-      <c r="B47" s="0"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
-      <c r="B48" s="0"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
-      <c r="B49" s="0"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
-      <c r="B50" s="0"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
@@ -649,219 +1027,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="26.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="26.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="3" width="26.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="3"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="3"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="3"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="3"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="3"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="3"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="3"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="3"/>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -881,396 +1094,396 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:E10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>

</xml_diff>